<commit_message>
checked for sign error typos in AS, BC, Kosice, CB, SC (events with large radiant diffs) radiant azimuths and flipped signs for AS and SC to make them match the ground-based measurements more: reran the notebook with the new radiant diffs for the new azimuths: made notes: added original sat-ecf excel sheet
</commit_message>
<xml_diff>
--- a/speed_radiant_difference/sat-ecf-local-sep-5-2017.xlsx
+++ b/speed_radiant_difference/sat-ecf-local-sep-5-2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\oldE\fireballs\Satellite Data\JPL-bolide-reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Projects\Thesis\speed_radiant_difference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9698E5BE-38CF-4357-B692-3E6F546C8FF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA156B58-AD77-45D5-B1A3-48E9C7E8382F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="870" windowWidth="32835" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,9 +192,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,26 +227,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,26 +262,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,7 +441,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>-10.8</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -514,13 +480,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>16.8</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3">
-        <v>1.2</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -528,13 +494,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>59.8</v>
+        <v>39.1</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4">
-        <v>-12.8</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -542,7 +508,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>36</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -554,7 +520,7 @@
         <v>18</v>
       </c>
       <c r="F5">
-        <v>49.3</v>
+        <v>39.1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -563,7 +529,7 @@
       </c>
       <c r="C6">
         <f>-F2*SIN(B4*J1)*COS(B3*J1)-F3*SIN(J1*B3)*SIN(J1*B4)+F4*COS(B4*J1)</f>
-        <v>2.197362090477192</v>
+        <v>-23.896733891078426</v>
       </c>
       <c r="D6">
         <v>0.1</v>
@@ -572,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="F6">
-        <v>-116.9</v>
+        <v>40.200000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -581,7 +547,7 @@
       </c>
       <c r="C7">
         <f>-F2*SIN(B3*J1)+F3*COS(B3*J1)</f>
-        <v>4.2703268039550322</v>
+        <v>2.6700973661016238</v>
       </c>
       <c r="D7">
         <v>0.1</v>
@@ -593,7 +559,7 @@
       </c>
       <c r="C8">
         <f>-F2*COS(B4*J1)*COS(B3*J1)-F3*COS(B4*J1)*SIN(J1*B3)-F4*SIN(B4*J1)</f>
-        <v>16.088999621814803</v>
+        <v>-0.86411191087774952</v>
       </c>
       <c r="D8">
         <v>0.1</v>
@@ -610,7 +576,7 @@
       </c>
       <c r="D10">
         <f>ATAN2(C6,C7)/J1+180</f>
-        <v>242.77122043578342</v>
+        <v>353.62451034489607</v>
       </c>
       <c r="E10" s="1">
         <f>((C6^2*D7^2+C7^2*D6^2)/(C6^2+C7^2))^0.5</f>
@@ -623,7 +589,7 @@
       </c>
       <c r="D11">
         <f>ATAN((C6^2+C7^2)^0.5/C8)/J1</f>
-        <v>16.620176150558713</v>
+        <v>-87.941869081399204</v>
       </c>
       <c r="F11">
         <v>23.841359763572328</v>
@@ -635,7 +601,7 @@
       </c>
       <c r="D12">
         <f>(F2^2+F3^2+F4^2)^0.5</f>
-        <v>16.790473489452289</v>
+        <v>24.060964236705065</v>
       </c>
       <c r="E12">
         <v>0.8</v>

</xml_diff>